<commit_message>
Added several epics to backlog
</commit_message>
<xml_diff>
--- a/Team_8_CS499/CS499_Backlog.xlsx
+++ b/Team_8_CS499/CS499_Backlog.xlsx
@@ -7,22 +7,20 @@
     <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Backlog" sheetId="1" r:id="rId1"/>
+    <sheet name="Options" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="Developers">Options!$A$4:$A$6</definedName>
+    <definedName name="Status">Options!$A$1:$A$2</definedName>
+  </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
-  <si>
-    <t>I want</t>
-  </si>
-  <si>
-    <t>so that</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="47">
   <si>
     <t>#</t>
   </si>
@@ -43,6 +41,126 @@
   </si>
   <si>
     <t>Assigned to</t>
+  </si>
+  <si>
+    <t>So that…</t>
+  </si>
+  <si>
+    <t>I want…</t>
+  </si>
+  <si>
+    <t>To be able to manually input Instructors</t>
+  </si>
+  <si>
+    <t>To be able to manually input Courses</t>
+  </si>
+  <si>
+    <t>To be able to manually input Rooms/Buildings</t>
+  </si>
+  <si>
+    <t>A course schedule can be created and modified</t>
+  </si>
+  <si>
+    <t>A course schedule can be created and modified with the quickest possible method</t>
+  </si>
+  <si>
+    <t>To see a course schedule automatically created</t>
+  </si>
+  <si>
+    <t>The scheduling process becomes quicker and easier</t>
+  </si>
+  <si>
+    <t>To see a list of conflicts or other situations where manual intervention may be required</t>
+  </si>
+  <si>
+    <t>Discretion can be used to set the schedule accordingly</t>
+  </si>
+  <si>
+    <t>To have minimum disruption of current scheduling procedures</t>
+  </si>
+  <si>
+    <t>The schedule can be created smoothly and accurately</t>
+  </si>
+  <si>
+    <t>To be able to manually input instructor/course preferences/priorities</t>
+  </si>
+  <si>
+    <t>To allow ease of use among multiple departments</t>
+  </si>
+  <si>
+    <t>To have an easy to use, intuitive GUI</t>
+  </si>
+  <si>
+    <t>To have the ability to produce comma/tab deliminited data files that can be read with Microsoft Excel</t>
+  </si>
+  <si>
+    <t>The outputs can be provided to the Dean for final approval of the schedule</t>
+  </si>
+  <si>
+    <t>To be able to import all of my course/instructor/preference information with a comma delimited file</t>
+  </si>
+  <si>
+    <t>Open</t>
+  </si>
+  <si>
+    <t>Closed</t>
+  </si>
+  <si>
+    <t>To create an easy to use GUI interface</t>
+  </si>
+  <si>
+    <t>To parse an input .csv format file</t>
+  </si>
+  <si>
+    <t>To develop a .csv file output object</t>
+  </si>
+  <si>
+    <t>To develop the ability to add instructors</t>
+  </si>
+  <si>
+    <t>To develop the ability to add courses</t>
+  </si>
+  <si>
+    <t>To develop the ability to add rooms/buildings</t>
+  </si>
+  <si>
+    <t>To develop an automatic course scheduling algorithm</t>
+  </si>
+  <si>
+    <t>It will speed the creation of department schedules</t>
+  </si>
+  <si>
+    <t>It satisfies the needs of the users and is easy to use</t>
+  </si>
+  <si>
+    <t>All instructors, courses, and preferences can be loaded simultaniously rather than manually</t>
+  </si>
+  <si>
+    <t>Users can output a Microsoft Excel readable file</t>
+  </si>
+  <si>
+    <t>The scheduling algorithm can use these objects as well as having the ability to manually add them</t>
+  </si>
+  <si>
+    <t>Manecke</t>
+  </si>
+  <si>
+    <t>Webb</t>
+  </si>
+  <si>
+    <t>Eccleston</t>
+  </si>
+  <si>
+    <t>To have a precompiled list of courses and teachers</t>
+  </si>
+  <si>
+    <t>The program can read the list and create a schedule</t>
+  </si>
+  <si>
+    <t>To print the course schedule</t>
+  </si>
+  <si>
+    <t>The schedule can be distributed to teachers or kept for reference</t>
   </si>
 </sst>
 </file>
@@ -79,7 +197,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -102,18 +220,159 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -410,68 +669,431 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="18.28515625" customWidth="1"/>
-    <col min="3" max="3" width="19.5703125" customWidth="1"/>
-    <col min="4" max="4" width="18.140625" customWidth="1"/>
-    <col min="5" max="5" width="22.28515625" customWidth="1"/>
-    <col min="7" max="7" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="14" style="1" customWidth="1"/>
+    <col min="3" max="3" width="38.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="42.85546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="22.28515625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="6.7109375" style="9" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="F1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="G1" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="B2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="2"/>
+      <c r="F2" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="G2" s="2"/>
+    </row>
+    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="B5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>6</v>
+      <c r="B9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="F15" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>16</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="F17" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>17</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="F18" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>18</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="F19" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>19</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="F20" s="9" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="F1:F1048576">
+    <cfRule type="containsText" dxfId="5" priority="2" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",F1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="1" operator="containsText" text="Closed">
+      <formula>NOT(ISERROR(SEARCH("Closed",F1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="F2:F1048576">
+      <formula1>Status</formula1>
+    </dataValidation>
+    <dataValidation allowBlank="1" showInputMessage="1" sqref="F1:G1"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="G2:G1048576">
+      <formula1>Developers</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:A6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>